<commit_message>
Marcos: Enviando diretorio com a lista do tipo LESE + Alteracoes na tabela de comparacao
</commit_message>
<xml_diff>
--- a/Listas-comparacao.xlsx
+++ b/Listas-comparacao.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Senac\Dropbox\Mestrado\UDESC - PAA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projetos\PAA_mestrado\PAA-ContaSaltos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6206D051-7538-440E-B10D-4E1E51D2E71C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="8055"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,26 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Senac</author>
   </authors>
   <commentList>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -148,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -255,6 +247,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -264,8 +258,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -593,16 +585,15 @@
     <col min="4" max="4" width="10.875" style="3"/>
     <col min="5" max="5" width="5.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="5.875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -621,30 +612,30 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -692,7 +683,9 @@
       <c r="G9" s="1">
         <v>10000</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>10000</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
@@ -713,15 +706,17 @@
       <c r="G10" s="1">
         <v>5999</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <v>3000</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E11" s="8"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="7"/>
+      <c r="E12" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>